<commit_message>
Carga completa actividades json
</commit_message>
<xml_diff>
--- a/public/data/excel/actividades.xlsx
+++ b/public/data/excel/actividades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="535">
   <si>
     <t>PROVINCIA</t>
   </si>
@@ -79,6 +79,48 @@
     <t>Jujuy</t>
   </si>
   <si>
+    <t>La Pampa</t>
+  </si>
+  <si>
+    <t>La Rioja</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t>Misiones</t>
+  </si>
+  <si>
+    <t>Neuquén</t>
+  </si>
+  <si>
+    <t>Río Negro</t>
+  </si>
+  <si>
+    <t>Salta</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>San Luis</t>
+  </si>
+  <si>
+    <t>Santa Cruz</t>
+  </si>
+  <si>
+    <t>Santa Fe</t>
+  </si>
+  <si>
+    <t>Santiago del Estero</t>
+  </si>
+  <si>
+    <t>Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Tucumán</t>
+  </si>
+  <si>
     <t>buenos_aires</t>
   </si>
   <si>
@@ -109,6 +151,48 @@
     <t>jujuy</t>
   </si>
   <si>
+    <t>la_pampa</t>
+  </si>
+  <si>
+    <t>la_rioja</t>
+  </si>
+  <si>
+    <t>mendoza</t>
+  </si>
+  <si>
+    <t>misiones</t>
+  </si>
+  <si>
+    <t>neuquen</t>
+  </si>
+  <si>
+    <t>rio_negro</t>
+  </si>
+  <si>
+    <t>salta</t>
+  </si>
+  <si>
+    <t>san_juan</t>
+  </si>
+  <si>
+    <t>san_luis</t>
+  </si>
+  <si>
+    <t>santa_cruz</t>
+  </si>
+  <si>
+    <t>santa_fe</t>
+  </si>
+  <si>
+    <t>santiago_del_estero</t>
+  </si>
+  <si>
+    <t>tierra_del_fuego</t>
+  </si>
+  <si>
+    <t>tucuman</t>
+  </si>
+  <si>
     <t>Conocer la tradición gauchesca y criolla</t>
   </si>
   <si>
@@ -197,6 +281,132 @@
   </si>
   <si>
     <t>Caminar por un desierto de sal</t>
+  </si>
+  <si>
+    <t>Saborear los vinos pampeanos</t>
+  </si>
+  <si>
+    <t>Conocer las salinas pampeanas</t>
+  </si>
+  <si>
+    <t>Visitar el Museo El Castillo</t>
+  </si>
+  <si>
+    <t>Visitar los museos de la ciudad</t>
+  </si>
+  <si>
+    <t>Conducir por la Cuesta de Miranda</t>
+  </si>
+  <si>
+    <t>Vivir la Chaya</t>
+  </si>
+  <si>
+    <t>Seguir los pasos del General San Martín</t>
+  </si>
+  <si>
+    <t>Hacer rafting en el Río Atuel</t>
+  </si>
+  <si>
+    <t>Esquiar en el Valle de Las Leñas</t>
+  </si>
+  <si>
+    <t>Conocer las minas de Wanda</t>
+  </si>
+  <si>
+    <t>Conocer las Cataratas del Iguazú</t>
+  </si>
+  <si>
+    <t>Acampar en la naturaleza</t>
+  </si>
+  <si>
+    <t>Bucear en el bosque sumergido</t>
+  </si>
+  <si>
+    <t>Descansar en las termas de Copahue</t>
+  </si>
+  <si>
+    <t>Conocer el Parque Vía Christi</t>
+  </si>
+  <si>
+    <t>Realizar trekking por el río Azul</t>
+  </si>
+  <si>
+    <t>Esquiar y realizar snowboard en el cerro Catedral</t>
+  </si>
+  <si>
+    <t>Navegar por el lago Nahuel Huapi</t>
+  </si>
+  <si>
+    <t>Remar en el Río Juramento</t>
+  </si>
+  <si>
+    <t>Viajar a las nubes en tren</t>
+  </si>
+  <si>
+    <t>Fotografiar los salares en la puna</t>
+  </si>
+  <si>
+    <t>Practicar kitesurf y el windsurf</t>
+  </si>
+  <si>
+    <t>Navegar en kayak por el río San Juan</t>
+  </si>
+  <si>
+    <t>Caminar por el Valle de la Luna</t>
+  </si>
+  <si>
+    <t>Realizar actividades náuticas</t>
+  </si>
+  <si>
+    <t>Recorrer el circuito histórico La Punta</t>
+  </si>
+  <si>
+    <t>Disfrutar del Dique Luján</t>
+  </si>
+  <si>
+    <t>Avistar pingüinos penacho amarillo y toninas overas</t>
+  </si>
+  <si>
+    <t>Caminar sobre el glaciar Perito Moreno</t>
+  </si>
+  <si>
+    <t>Hacer trekking en El Chaltén</t>
+  </si>
+  <si>
+    <t>Visitar la cuna de nuestra bandera</t>
+  </si>
+  <si>
+    <t>Navegar por el río Paraná</t>
+  </si>
+  <si>
+    <t>Recorrer la historia de la ciudad de Santa Fe</t>
+  </si>
+  <si>
+    <t>Relajarse en Termas de Río Hondo</t>
+  </si>
+  <si>
+    <t>Vivir la adrenalina en el autódromo</t>
+  </si>
+  <si>
+    <t>Vivir el folklore en el Patio del Indio Froilán</t>
+  </si>
+  <si>
+    <t>Esquiar y realizar snowboard en el fin del mundo</t>
+  </si>
+  <si>
+    <t>Navegar por el Canal de Beagle</t>
+  </si>
+  <si>
+    <t>Recorrer el norte fueguino</t>
+  </si>
+  <si>
+    <t>Recorrer la Ruta del Artesano</t>
+  </si>
+  <si>
+    <t>Caminar por la Ciudad Sagrada de Quilmes</t>
+  </si>
+  <si>
+    <t>Remar en el dique El Cadillal</t>
   </si>
   <si>
     <t>San Antonio de Areco, provincia de Buenos Aires</t>
@@ -302,6 +512,150 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">La Pampa
+</t>
+  </si>
+  <si>
+    <t>Salinas Grandes de Hidalgo, La Pampa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Museo Castillo, Parque Luro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Rioja capital
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta 40, La Rioja
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Rioja capital, La Rioja
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los Chacayes, Mendoza
+</t>
+  </si>
+  <si>
+    <t>Río Atuel</t>
+  </si>
+  <si>
+    <t>Valle de Las Leñas</t>
+  </si>
+  <si>
+    <t>Wanda, Misiones</t>
+  </si>
+  <si>
+    <t>Iguazú, Misiones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campo Ramón, Misiones
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lago Traful, Neuquén
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copahue, Neuquén
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junín de los Andes, Neuquén
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Bolsón, Río Negro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Carlos de Bariloche, Río Negro
+</t>
+  </si>
+  <si>
+    <t>Nahuel Huapi, Rio Negro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coronel Moldes, Salta
+</t>
+  </si>
+  <si>
+    <t>San Antonio de los Cobres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tolar Grande, Salta
+</t>
+  </si>
+  <si>
+    <t>Rodeo, San Juan</t>
+  </si>
+  <si>
+    <t>San Juan ciudad</t>
+  </si>
+  <si>
+    <t>Parque Provincial Ischigualasto, San Juan</t>
+  </si>
+  <si>
+    <t>La Florida, San Luis</t>
+  </si>
+  <si>
+    <t>La Punta, San Luis</t>
+  </si>
+  <si>
+    <t>Luján, San Luis</t>
+  </si>
+  <si>
+    <t>Puerto Deseado, Santa Cruz</t>
+  </si>
+  <si>
+    <t>Parque Nacional Los Glaciares, Santa Cruz</t>
+  </si>
+  <si>
+    <t>El Chaltén</t>
+  </si>
+  <si>
+    <t>Rosario, Santa Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosario, Santa Fe
+</t>
+  </si>
+  <si>
+    <t>Manzana Jesuítica de Santa Fe</t>
+  </si>
+  <si>
+    <t>Termas de Rio Hondo, Santiago del Estero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termas de Rio Hondo, Santiago del Estero
+</t>
+  </si>
+  <si>
+    <t>Patio del Indio Froilán, Ciudad de Santiago del Etero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ushuaia, Tierra del Fuego AIAS
+</t>
+  </si>
+  <si>
+    <t>Isla de los Pájaros,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En Río Grande, Tierra del Fuego AIAS
+</t>
+  </si>
+  <si>
+    <t>Valles Calchaquíes, Tucumán</t>
+  </si>
+  <si>
+    <t>Ruta 40, Tucumán</t>
+  </si>
+  <si>
+    <t>dique El Cadillal</t>
+  </si>
+  <si>
     <t>/img/actividades/bs/bs1/1.png</t>
   </si>
   <si>
@@ -392,6 +746,132 @@
     <t>/img/actividades/jujuy/7.png</t>
   </si>
   <si>
+    <t>/img/actividades/la-pampa/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/7.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/1.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/4.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/7.png</t>
+  </si>
+  <si>
     <t>/img/actividades/bs/bs1/2.png</t>
   </si>
   <si>
@@ -482,6 +962,132 @@
     <t>/img/actividades/jujuy/8.png</t>
   </si>
   <si>
+    <t>/img/actividades/la-pampa/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/8.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/2.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/5.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/8.png</t>
+  </si>
+  <si>
     <t>/img/actividades/bs/bs1/3.png</t>
   </si>
   <si>
@@ -572,125 +1178,671 @@
     <t>/img/actividades/jujuy/9.png</t>
   </si>
   <si>
-    <t>Conocer la tradición gauchesca y criolla en San Antonio de Areco, provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Aprender sobre arquitectura moderna en La Plata, Provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Pasear en una isla con historia en Isla Martín García, provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Conectarse con el cielo en el Planetario de la Ciudad en Buenos Aires Ciudad es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Conocer el legado del General San Martín en Buenos Aires Ciudad es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Vivir la magia del Teatro Colón en Paso obligado en la ciudad, reconocida arquitectura y acústica única es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Explorar la Cordillera de los Andes en Fiambalá, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Visitar museos de historia y arte en San Fernando del Valle de Catamarca, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Explorar el Pueblo Perdido de la Quebrada en San Fernando del Valle de Catamarca, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Disfrutar las aguas termales en Presidencia Roque Sáez Peña, Chaco
- es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Conocer los meteoritos en el campo del cielo en Secretos del cielo y de los meteoritos en Gancedo
- es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Pescar en la Isla del Cerrito en Isla del Cerrito, Chaco es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Esquiar fuera de pista en La Hoya en Cerro La Hoya, Esquel, Chubut
- es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Viajar en el tren La Trochita en Esquel y El Maitén, Chubut
- es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Avistar ballenas en Península Valdés en Disfrutar las ballenas y sentir la naturaleza viva
- es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Descubrir la cultura de la docta en Ciudad de Córdoba
- es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Disfrutar del río en el Valle de Traslasierra en Nono y Mina Clavero, Córdoba es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Visitar las estancias jesuíticas en Conocer el gran legado histórico cultural jesuita
- es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Descubrir la armonía entre naturaleza y comunidad en Concepción del Yaguareté Corá, Corrientes
- es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Conocer los comienzos del General San Martin en Yapeyú, Corrientes
- es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Descubrir paisajes y fósiles en el sur de Corrientes en Empedrado y Bella Vista, Corrientes
- es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Conocer el carnaval y sus colores en Gualeguaychú, Entre Ríos
- es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Disfrutar los beneficios de las Termas en Relajarse, recuperar el bienestar y contemplar el entorno
- es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Caminar en el Parque Nacional El Palmar en Senderos, canto de aves y palmeras Butia yatay
- es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Hacer un safari fotográfico en el Bañado La Estrella en Explorar los bañados, navegar y observar flora y fauna
- es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Degustar la gastronomía formoseña en Sabores que nacen del río y del monte
- es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Caminar por las pasarelas del Parque Nacional Río Pilcomayo en Laguna Blanca, Formosa
- es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Recorrer la selva de montaña en Calilegua, Jujuy
- es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Viajar al Valle de la Luna jujeño en Ruta 40, Jujuy
- es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Caminar por un desierto de sal en La belleza incomparable de la inmensidad
- es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.</t>
-  </si>
-  <si>
-    <t>Es una experiencia ideal para quienes disfrutan del turismo cultural, el contacto con las tradiciones locales y la posibilidad de aprender mientras recorren. Perfecta para sumar contexto y profundidad al viaje.</t>
-  </si>
-  <si>
-    <t>Es una actividad versátil que se adapta a distintos tipos de viajeros, aportando una experiencia enriquecedora y auténtica. Una excelente opción para completar una escapada y conocer el lugar en profundidad.</t>
-  </si>
-  <si>
-    <t>Pensada para quienes buscan desconectar de la rutina y acercarse a la naturaleza, esta actividad permite vivir el destino desde un lugar más sensorial y tranquilo. Ideal para disfrutar sin apuros.</t>
-  </si>
-  <si>
-    <t>La propuesta invita a disfrutar del paisaje y del ritmo propio del lugar, ideal para quienes buscan una experiencia relajada, visual y conectada con el entorno. Aporta una mirada distinta y memorable del destino.</t>
+    <t>/img/actividades/la-pampa/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-pampa/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/la-rioja/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/mendoza/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/misiones/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/neuquen/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/rio-negro/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/salta/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-juan/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/san-luis/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-cruz/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santa-fe/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/santiago-del-estero/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tierra-del-fuego/9.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/3.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/6.png</t>
+  </si>
+  <si>
+    <t>/img/actividades/tucuman/9.png</t>
+  </si>
+  <si>
+    <t>Conocer la tradición gauchesca y criolla en San Antonio de Areco, provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Aprender sobre arquitectura moderna en La Plata, Provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita
+a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Pasear en una isla con historia en Isla Martín García, provincia de Buenos Aires es una actividad destacada dentro de la oferta turística de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta
+invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Conectarse con el cielo en el Planetario de la Ciudad en Buenos Aires Ciudad es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.
+Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Conocer el legado del General San Martín en Buenos Aires Ciudad es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Vivir la magia del Teatro Colón en Paso obligado en la ciudad, reconocida arquitectura y acústica única es una actividad destacada dentro de la oferta turística de Ciudad Autónoma de Buenos Aires. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven
+único dentro de la provincia. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una
+forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Explorar la Cordillera de los Andes en Fiambalá, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el
+lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Visitar museos de historia y arte en San Fernando del Valle de Catamarca, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta
+invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Explorar el Pueblo Perdido de la Quebrada en San Fernando del Valle de Catamarca, Catamarca es una actividad destacada dentro de la oferta turística de Catamarca. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Disfrutar las aguas termales en Presidencia Roque Sáez Peña, Chaco  es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir
+el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Conocer los meteoritos en el campo del cielo en Secretos del cielo y de los meteoritos en Gancedo  es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Pescar en la Isla del Cerrito en Isla del Cerrito, Chaco es una actividad destacada dentro de la oferta turística de Chaco. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el lugar
+desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Esquiar fuera de pista en La Hoya en Cerro La Hoya, Esquel, Chubut  es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir
+el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Viajar en el tren La Trochita en Esquel y El Maitén, Chubut  es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el
+lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Avistar ballenas en Península Valdés en Disfrutar las ballenas y sentir la naturaleza viva  es una actividad destacada dentro de la oferta turística de Chubut. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Descubrir la cultura de la docta en Ciudad de Córdoba  es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el lugar
+desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Disfrutar del río en el Valle de Traslasierra en Nono y Mina Clavero, Córdoba es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Visitar las estancias jesuíticas en Conocer el gran legado histórico cultural jesuita  es una actividad destacada dentro de la oferta turística de Córdoba. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta
+invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Descubrir la armonía entre naturaleza y comunidad en Concepción del Yaguareté Corá, Corrientes  es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia.
+Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Conocer los comienzos del General San Martin en Yapeyú, Corrientes  es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Descubrir paisajes y fósiles en el sur de Corrientes en Empedrado y Bella Vista, Corrientes  es una actividad destacada dentro de la oferta turística de Corrientes. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Conocer el carnaval y sus colores en Gualeguaychú, Entre Ríos  es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir
+el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Disfrutar los beneficios de las Termas en Relajarse, recuperar el bienestar y contemplar el entorno  es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la
+provincia. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y
+auténtica.</t>
+  </si>
+  <si>
+    <t>Caminar en el Parque Nacional El Palmar en Senderos, canto de aves y palmeras Butia yatay  es una actividad destacada dentro de la oferta turística de Entre Rios. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Hacer un safari fotográfico en el Bañado La Estrella en Explorar los bañados, navegar y observar flora y fauna  es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la
+provincia. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y
+auténtica.</t>
+  </si>
+  <si>
+    <t>Degustar la gastronomía formoseña en Sabores que nacen del río y del monte  es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Caminar por las pasarelas del Parque Nacional Río Pilcomayo en Laguna Blanca, Formosa  es una actividad destacada dentro de la oferta turística de Formosa. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta
+invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Recorrer la selva de montaña en Calilegua, Jujuy  es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el lugar desde una
+primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Viajar al Valle de la Luna jujeño en Ruta 40, Jujuy  es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a descubrir el lugar desde
+una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Caminar por un desierto de sal en La belleza incomparable de la inmensidad  es una actividad destacada dentro de la oferta turística de Jujuy. Permite recorrer el lugar con calma, conocer su historia, su entorno y los elementos que lo vuelven único dentro de la provincia. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La Pampa posee una propuesta enoturística que combina paisajes rurales, sabores únicos y el espíritu emprendedor de sus comunidades. El recorrido atraviesa viñedos, bodegas y proyectos familiares o comunales distribuidos entre la capital provincial, la región centro-sur y la costa del río Colorado.
+Además de degustaciones, se pueden realizar caminatas por los viñedos, paseos en bicicleta, participar de cosechas y conocer chacras donde también se cultivan frutales, olivos y frutos secos. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su
+identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Ubicadas en los valles del sureste, estas extensas planicies blancas permiten conocer el proceso de extracción de la sal común y descubrir historias locales únicas. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace
+especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Museo El Castillo se encuentra dentro de la Reserva Provincial Parque Luro, en La Pampa. Es una antigua casona de estilo francés construida a principios del siglo XX que conserva su mobiliario original y fue declarada Monumento Histórico Nacional. Esta propuesta invita a descubrir el lugar desde
+una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Las tradiciones y la música folklórica permanecen vivas en las costumbres riojanas. El Museo Folklórico es una casa antigua, decorada con piezas únicas y con una gran variedad de instrumentos. También se pueden conocer las manufacturas típicas de la provincia en el Mercado Artesanal. Elementos de
+uso cotidiano y ornamental se exponen y están a la venta, dando apoyo a los artesanos. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el
+contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Este espectacular tramo de la legendaria Ruta 40 tiene una de las cuestas más hermosas de la Argentina. Entre Villa Unión y Chilecito, el camino de cornisa (asfaltado) asciende hasta los 2040 msnm y regala vistas increíbles. La experiencia suele complementarse con el sobrevuelo de cóndores. El río
+Miranda acompaña a la ruta bordeándola por un valle en el que el verde de los montes y cardones contrasta con los rojos, ocres y naranjas del suelo. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una
+excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La invitación es a vivir la magia del Carnaval de la Chaya, una celebración ancestral que honra a la Pachamama y que llena las calles riojanas de harina, albahaca, música y alegría. Allí se puede conocer la leyenda del Pujllay, espíritu juguetón y festivo que simboliza la unión entre el pueblo y la
+naturaleza, y que cada año renace en los festejos hasta su quema final, rito que marca despedir el carnaval. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el
+recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Los Chacayes, en Tunuyán, Mendoza, es conocido por la pureza de su agua, su producción enológica y su historia vinculada al paso del General San Martín y a la preservación de la naturaleza. La propuesta es visitar el Parque Temático Manzano Histórico, con el monumento Retorno a la Patria, el Paseo
+Vida y Obra del General San Martín, y los museos Retorno a la Patria y Arqueológico y de Ciencias Naturales. También, conocer el Manzano Histórico, árbol bajo el cual San Martín descansó en 1823 tras la gesta libertadora, preservado por más de dos siglos y declarado Árbol Histórico Nacional. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Desde Valle Grande, a 30 kilómetros de la ciudad de San Rafael parten las excursiones de rafting en gomones. Los recorridos varían en distancias y en tiempo, y son aptos para todo público. Los llamados “rápidos del Atuel” invitan a vivir el río a través de la aventura. En la zona hay prestadores
+especializados en esta actividad y otras afines. Durante el verano el río baja con mayor caudal y los rápidos se vuelven más intensos y divertidos. En invierno, el caudal y la velocidad son menores, ideal para contemplar el paisaje del cañón y hacer kayak o navegar. Esta propuesta invita a descubrir
+el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>En plena Cordillera de los Andes y a 80 km de Malargüe se encuentra Las Leñas, un centro de ski de alta montaña con base en los 2240 msnm y cumbre en los 3430 msnm. El centro cuenta con opciones de esquí y snowboard para principiantes y experimentados, y además ofrecen ski adaptado. También tienen
+una experiencia única, practicar esquí nocturno. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del
+destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>A 51 kilómetros de Puerto Iguazú este lugar ubicado en la localidad de Wanda es famoso por su riqueza en piedras semipreciosas, como ágatas, amatistas, topacios, cuarzos y jaspes, que brillan en los túneles y galerías subterráneas. Es posible encontrar venta de artesanías realizadas con ellas en
+toda la provincia. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana
+y auténtica.</t>
+  </si>
+  <si>
+    <t>Ubicadas dentro del Parque Nacional Iguazú, fueron declaradas Patrimonio Mundial por la UNESCO. Son una de las Siete Maravillas Naturales del Mundo y un destino que hay que visitar al menos una vez en la vida. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su
+entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Campo Ramón, a 115 kilómetros de Posadas, se destaca particularmente por su variada oferta de campings inmersos en un paisaje de naturaleza y del monte nativo, todos ellos situados a orillas de arroyos y/o saltos de agua. Sus cuencas hídricas son las protagonistas, como el arroyo El Bonito, el Ramón
+o el Acaraguá, que proveen el caudal para las actividades acuáticas y la frescura natural que buscan los visitantes. Uno de los saltos de agua más reconocidos es el Teodoro Cuenca, con una caída de 15 metros. Allí se puede descansar y refrescarse. Esta propuesta invita a descubrir el lugar desde una
+primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Lago Traful es uno de los famosos siete lagos de la Ruta 40, ubicado dentro del Parque Nacional Nahuel Huapi, en Neuquén. A 30 metros de profundidad, el bosque sumergido deslumbra y ofrece vistas únicas a quienes se animen a bucear entre gigantescos cipreses casi intactos. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>A solo 17 km de Caviahue, por un camino de ripio, se encuentra Copahue, un complejo termal único, famoso por la calidad y variedad de sus aguas, fangos y algas. Ubicadas al pie del volcán Copahue, estas termas son las únicas en el mundo que combinan en un mismo lugar una increíble diversidad de
+recursos minerales naturales. Con más de 20 tipos de aguas mineromedicinales, ofrecen un entorno ideal para la relajación y el bienestar. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente
+oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Parque Escultórico Temático Vía Christi, es un parque de 2 kilómetros ubicado en Junín de los Andes, que retrata los momentos más importantes de la vida de Jesucristo a través de 24 estaciones. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su
+identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Área Natural Protegida Río Azul - Lago Escondido, al oeste de El Bolsón, es el sitio ideal para hacer senderismo y trekking entre paisajes impresionantes. Este paraíso natural es uno de los rincones más espectaculares de la cordillera. Se puede disfrutar de cristalinos pozones de agua turquesa,
+con el Cajón del Río Azul como una de las principales atracciones. Recorrer la red de senderos de mediana y alta dificultad, que en muchas ocasiones se interconectan, es la actividad perfecta para los amantes del senderismo. Hay opciones de excursiones de un día o una experiencia más completa
+acampando o durmiendo en refugios de montaña. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del
+destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Ideal para disfrutar de la nieve argentina en el centro de esquí más grande y moderno del hemisferio sur. Próximo a la reconocida ciudad barilochense, tiene espectaculares vistas de los lagos y bosques del Parque Nacional Nahuel Huapi. Posee 1.200 hectáreas esquiables, 59 pistas con un máximo de
+largo de 9km y 30 medios de elevación, entre ellos la innovadora Telesilla séxtuple. Su desnivel esquiable es de 1.000 mts. entre la base y la cumbre para disfrutar de las mejores pendientes y un avanzado sistema de fabricación de nieve. Esta propuesta invita a descubrir el lugar desde una primera
+mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La navegación por el lago Nahuel Huapi es una de las excursiones imperdibles para quien visita el Parque Nacional Nahuel Huapi y la ciudad de San Carlos de Bariloche. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace
+especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El embalse General Belgrano y el dique Cabra Corral, despliegan un espejo de agua entre montañas verdes, donde comienza el río Juramento, escenario natural de excursiones y travesías en rafting. El descenso por sus rápidos, desde el dique hasta el paraje Los Lapachos (12 kilómetros de recorrido),
+revela un paisaje de paredes milenarias, formadas hace más de 65 millones de años. Una experiencia de intensidad media, con una duración aproximada de 2 horas, ideal para quienes buscan emociones en plena naturaleza. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en
+valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Tren a las Nubes es uno de los más altos del mundo y recorre los increíbles paisajes de la Puna salteña llegando hasta el Viaducto La Polvorilla, una magnífica obra de ingeniería a 4200 msnm. El reconocido Tren a las Nubes sale desde el pueblo de San Antonio de los Cobres y llega hasta el
+viaducto en un viaje de 1 hora y media en total, una experiencia cultural y paisajística única en el mundo. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el
+recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Tolar Grande está situado en la Puna, a 387 kilómetros de la ciudad de Salta. Está rodeado de volcanes y posee una belleza impactante. Ideales para la contemplación y la fotografía, las Salinas Grandes conforman extensos mares blancos que se pierden en el horizonte. El Salar de Arizaro es uno de los
+más grande de Sudamérica y alberga el imponente Cono de Arita, una pirámide natural de origen volcánico. El Desierto del Diablo se destaca por su aridez extrema y su inmensa planicie rojiza. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su
+identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Dique Cuesta del Viento es un lugar ideal para el desarrollo de estos deportes acuáticos por tener asegurados vientos fuertes más de 300 días al año. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una
+excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La propuesta es aventurarse en las aguas del río San Juan, rodeado de montañas, sol resplandeciente y cielos azules. Es un lugar perfecto para la práctica de kayak y elegido para competencias de este deporte nacionales e internacionales. Esta propuesta invita a descubrir el lugar desde una primera
+mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Parque Provincial Ischigualasto fue declarado Patrimonio Mundial por la UNESCO. Su importancia radica en el valor científico de los hallazgos paleontológicos realizados en el lugar ya que allí se han encontraron restos de algunos de los dinosaurios más antiguos del mundo. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La localidad y el embalse La Florida, cercano a El Trapiche y ubicado a 40 kilómetros de la ciudad de San Luis, es un destino ideal para quienes buscan disfrutar de la naturaleza y las actividades al aire libre. Su paisaje combina bosques, playas y un extenso espejo de agua, perfecto para la
+práctica de deportes náuticos durante todo el año. Entre las actividades destacadas se encuentran el esquí acuático, con clases disponibles para quienes deseen iniciarse, el Stand Up Paddle y el Windsurf. Además, sentarse en el muelle a contemplar el paisaje o las acrobacias de los deportistas sobre
+el agua son una experiencia relajante y entretenida. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia
+del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Esta ciudad moderna, pero cargada de simbolismo histórico, ofrece una propuesta turística diferente, donde la cultura y la innovación se entrelazan. Fundado el 26 de marzo de 2003, es el pueblo más joven de Argentina. Es posible ver el homenaje a los grandes hitos del pasado argentino como las
+réplicas del Cabildo de Buenos Aires y de la Casa Histórica de la Independencia de Tucumán. Permiten revivir momentos clave de nuestra historia en un entorno cuidadosamente diseñado. Recorrer estos espacios es como hacer un viaje en el tiempo, pero sin salir del presente. Locales del mismo estilo
+ofrecen servicio de cafetería y artesanías. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del
+destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Emplazado entre los imponentes cerros Independencia y Bandera se encuentra este dique el cual abarca una superficie de 27 hectáreas. A solo 3,6 kilómetros del ingreso a la localidad de Luján, en el departamento Ayacucho, se accede por la Ruta Nacional Nº 146 a este embalse fundado en 1958 sobre el
+río Luján. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y
+auténtica.</t>
+  </si>
+  <si>
+    <t>En los alrededores de Puerto Deseado se puede ver la única colonia continental de pingüinos penacho amarillo y navegar con las toninas overas, también conocidas como delfines patagónicos. Ambos son un símbolo de la Patagonia. Desde Puerto Deseado parten excursiones embarcadas para sentir la emoción
+de ver las toninas overas de cerca. Son muy curiosas y les gusta jugar próximas de los barcos. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido,
+entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Desde El Calafate se ingresa por tierra al parque nacional, para llegar al puerto Bajo de las Sombras y embarcarse en una navegación durante 20 minutos observando el frente cara sur del Glaciar Perito Moreno. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su
+entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Declarado por el Congreso Nacional como la “Capital Nacional del Trekking”, El Chaltén es un pueblo de montaña a los pies de los cerros Fitz Roy y Torre, a 220 kilómetros de El Calafate. Dos de sus senderos más conocidos: Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo
+en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Ciudad cosmopolita reconocida por sus propuestas musicales, teatrales, literarias e históricas. El punto de encuentro obligado de turistas y visitantes es el Parque de la Independencia, donde se encuentra el Monumento Histórico Nacional a la Bandera emplazado en el sitio donde el General Manuel
+Belgrano izó por primera vez la bandera nacional, el 27 de febrero de 1812. Desde su torre de 70 metros de altura se aprecian vistas panorámicas de la ciudad de Rosario, su costanera y el río Paraná. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno,
+su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Rosario es una ciudad que mira al río y ofrece diversas opciones para disfrutar su costa y practicar distintas actividades náuticas tales como pasear en lancha, gomón o velero, remar en kayak o hacer una excursión de pesca. Es posible realizar excursiones en barco por el río Paraná que permiten
+disfrutar de vistas de las costas de las islas y el puente Rosario-Victoria o ingresar al delta, recorriendo la zona de el Charigue y el Paraná Viejo. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es
+una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La ciudad de Santa Fe es la cuna de la Constitución Nacional. En 1853 se aprobó la Carta Magna y se sucedieron varios hechos históricos, cuyos vestigios y testimonios se pueden conocer a través del Parque y Museo de la Constitución Nacional. El ingreso es libre y gratuito. Esta propuesta invita a
+descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Termas de Río Hondo es un destino que se puede disfrutar durante todo el año, es ideal para quienes quieran relajar el cuerpo, la mente y disfrutar las bondades de sus aguas curativasEsta ciudad termal cuenta con establecimientos que ofrecen tratamientos de belleza, fangos y masajes, entre otras
+propuestas. Además cuentan con piscinas, spa al aire libre y actividades recreativas para todas las edades. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el
+recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Considerado como uno de los circuitos más modernos y prestigiosos de América Latina, es sede de competencias nacionales e internacionales que atraen visitantes de todo el mundo. El autódromo se encuentra a 6 kilómetros de Termas de Río Hondo. Algunos de los eventos deportivos que se pueden disfrutar
+en este predio son las distintas categorías del automovilismo argentino, tales como el Turismo Carretera, Súper TC 2000 y el Top Race. Además, para los amantes del motociclismo, una de las fechas más esperadas es el Gran Premio Internacional MotoGP que también tiene lugar en estas pistas. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Patio de Indio Froilán es un espacio de recreación cultural que recibe a turistas y santiagueños para disfrutar de buena música, comida típica y conocer al prestigioso y reconocido artesano de bombos. Este espacio que busca revalorizar las raíces de la provincia tuvo su origen en el año 1997
+cuando el propio Froilán organizó el cumpleaños de su sobrino y se juntó a guitarrear junto a unos amigos. Con el correr de los años se fue sumando más gente y llegó a albergar alrededor de mil personas y a convertirse en un ícono de la identidad local. Esta propuesta invita a descubrir el lugar
+desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>El Cerro Castor es el centro de esquí alpino más austral del mundo, donde también se puede practicar esquí de fondo, freestyle y snowboard; tanto para principiantes como para expertos de todas las edades. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su
+entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Desde el puerto de Ushuaia parten diariamente embarcaciones que recorren el Canal Beagle y sus paisajes emblemáticos. Las rutas clásicas incluyen la Isla de los Pájaros, la Isla de los Lobos y el faro Les Eclaireurs, donde es posible avistar aves y lobos marinos. Esta propuesta invita a descubrir el
+lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Río Grande ofrece diversos espacios naturales donde es posible explorar los ecosistemas característicos del norte fueguino. Entre sus sitios de interés se destacan Cabo Domingo y Cabo Peña, dos puntos con fuerte valor cultural e impresionantes panorámicas del océano Atlántico. Esta propuesta invita
+a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La Ruta del Artesano es un circuito del Valle Calchaquí ofrece al turista productos genuinos y originales hechos con materias nobles y naturales. También lo pone en contacto con la historia, la cultura y sus técnicas ancestrales. A lo largo de esta Ruta se pueden encontrar artesanías elaboradas con
+una amplia variedad de materias primas. En Tafí del Valle se observa el proceso ancestral del tejido en lana de oveja, teñida con tintes naturales y trabajada en telares criollos. En Amaicha del Valle se aprecia la cerámica pintada a mano y las artesanías en piedra con influencia diaguita. Esta
+propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>La Ciudad Sagrada de Quilmes está rodeada por los Valles Calchaquíes, a 17 kilómetros de Amaicha del Valle, sobre la mítica Ruta 40. Es uno de los principales sitios arqueológicos de la Argentina por ser el mayor asentamiento precolombino del país y último bastión de la resistencia indígena, además
+de por su magnitud y estado de conservación. Esta propuesta invita a descubrir el lugar desde una primera mirada, poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del
+destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Ubicado a solo 22 kilómetros de la capital de la provincia, este lugar invita a disfrutar de su imponente dique. Sus aguas son el escenario ideal para vivir la adrenalina del kayak, el canyoning y muchas más experiencias acuáticas. Esta propuesta invita a descubrir el lugar desde una primera mirada,
+poniendo en valor su entorno, su identidad y aquello que lo hace especial. Es una excelente oportunidad para comenzar el recorrido, entender el contexto y conectar con la esencia del destino de una forma cercana y auténtica.</t>
+  </si>
+  <si>
+    <t>Es una experiencia ideal para quienes disfrutan del turismo cultural, el contacto con las tradiciones locales y la posibilidad de aprender mientras recorren. Perfecta para sumar contexto y profundidad al viaje. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el
+tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Es una actividad versátil que se adapta a distintos tipos de viajeros, aportando una experiencia enriquecedora y auténtica. Una excelente opción para completar una escapada y conocer el lugar en profundidad. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo
+para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Pensada para quienes buscan desconectar de la rutina y acercarse a la naturaleza, esta actividad permite vivir el destino desde un lugar más sensorial y tranquilo. Ideal para disfrutar sin apuros. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para
+observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>La propuesta invita a disfrutar del paisaje y del ritmo propio del lugar, ideal para quienes buscan una experiencia relajada, visual y conectada con el entorno. Aporta una mirada distinta y memorable del destino. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el
+tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Esta experiencia permite al visitante conectarse con la tierra, aprender sobre procesos de producción local y disfrutar de una propuesta que crece con identidad propia en el corazón de la llanura pampeana. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo
+para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Los recorridos son peatonales y solo se realizan con guías habilitados para garantizar la seguridad y la protección del entorno. Hay distintos destinos para conocerlas: La Colorada Grande: a 43 kilómetros de General San Martín Salinas Grandes de Hidalgo: en Macachín Colorada Chica: a 30 kilómetros
+de Jacinto Arauz Salinas de Anzoátegui: en La Adela La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que
+deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>En su interior se pueden recorrer el salón principal, las caballerizas, el tambo y la sala de carruajes, entre otros espacios que permiten imaginar cómo era la vida en sus años de esplendor. Además de su valor arquitectónico, el lugar invita a conocer parte de la historia pampeana y la relación con
+los pueblos originarios que habitaron la zona. Rodeado por un entorno natural de caldenes y fauna autóctona, el museo es una parada ideal para quienes visitan el Parque Luro, combinando cultura, historia y naturaleza en un solo paseo. La experiencia se vive sin apuros, permitiendo disfrutar cada
+detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Para todos los gustos el Paseo Cultural Castro Barros alberga desde dinosaurios en la Sala Paleontológica, hasta Tienda de Artesanías y Café Literario, pasando por las salas de Arte Contemporáneo ó de Historia. Para cerrar el día se puede tomar el bus turístico que ofrece un recorrido de dos horas
+con guía. Se aprecian desde la parte superior del bus vistas panorámicas de los edificios emblemáticos y de los parques de la ciudad. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la
+zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>En su recorrido pasa por una quebrada conocida como La Pelea, donde en 1867 se atrincheraron fuerzas militares durante una batalla. Otra alternativa, para adentrarse más en el paisaje de la Cuesta de Miranda, es la experiencia única de recorrerla en bici. La experiencia se vive sin apuros,
+permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>La tradición implica recorrer los barrios para ver comparsas a caballo, escuchar vidalas y coplas, y participar del tradicional topamiento y la coronación, ceremonias donde compadres y comadres sellan su amistad intercambiando coronas de masa o flores bajo arcos adornados. Sentir la harina que
+simboliza la abundancia de la cosecha y la albahaca, perfumando los festejos como amuleto de alegría y protección. Descubrir un carnaval único en el país, donde la herencia diaguita convive con la espiritualidad de la tierra y el fervor popular. Vivir la Chaya es vivir La Rioja: un encuentro
+intenso, colorido y auténtico que invita a volver cada febrero. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una
+actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Recorrer el Museo Municipal Retorno a la Patria permite apreciar una muestra sanmartiniana en sus cuatro salas temáticas, con la posibilidad de realizar visitas guiadas o autoguiadas. Una actividad más intensa es realizar el Cruce de los Andes por el paso Portillo Piuquenes, a caballo o a pie, para
+contemplar los mismos paisajes que vieron San Martín y Darwin en su paso por la región. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan
+redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>La ruta provincial 173 une San Rafael con la zona de los rápidos del río Atuel y los diques-embalses Valle Grande y El Nihuil, en un recorrido de 85 kilómetros en total. Al pasar por el impresionante Cañón del Atuel se ven paredones que pueden llegar a los 260 metros de altura. Es un paisaje
+imponente con formaciones coloridas talladas por el viento y las aguas del río Atuel. Vale la pena hacerlo con tiempo para detenerse a admirar el paisaje. La ciudad de San Rafael cuenta con opciones de hospedajes de diferentes categorías, además de servicios. En la zona de Valle Grande y en Villa El
+Nihuil hay campings, cabañas, hoteles, restaurantes y proveedurías. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es
+una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>En Las Leñas hay diferentes propuestas de alojamiento para vivir en la montaña de día y de noche. Para las familias hay un parque de aventura con juegos y trineos. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal
+tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Las minas de piedras semipreciosas de Wanda son una maravilla geológica que invita a los visitantes a explorar su interior. Posee túneles y galerías donde se puede ver el proceso de extracción y pulido de las gemas y conocer su formación a lo largo de millones de años. Las minas no solo son un
+atractivo turístico por su valor geológico, sino también por el entorno natural de paisajes que combinan la serenidad del lugar con el esplendor de las gemas. Es una propuesta imperdible para quienes buscan una experiencia única y auténtica en el corazón de Misiones. La experiencia se vive sin
+apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Con sus 275 saltos, se pueden contratar salidas en gomón y en lancha que remontan el río hasta la base de las cascadas para sentir la fuerza increíble de los saltos (es importante llevar piloto o capa impermeable durante esta actividad). Si se prefiere navegar con más calma, hay paseos embarcados
+por el Iguazú Superior, con la posibilidad de observar la flora y fauna de la región. Si el viaje coincide con los días de luna llena, es posible disfrutar las pasarelas, los saltos de agua y los ruidos de la selva a la luz de la luna. Es una experiencia única que debe reservarse con tiempo. La
+experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho
+después del viaje.</t>
+  </si>
+  <si>
+    <t>Muchos de los campings de la zona complementan la experiencia agreste con otras comodidades como cabañas o piscinas abastecidas con la misma agua natural que fluye de los arroyos. Los visitantes tienen la oportunidad de recorrer una cooperativa productora de yerba mate para conocer en detalle el
+proceso de elaboración de esta infusión típica. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja
+recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Los árboles se mantienen en excelente estado debido a las bajas temperaturas del agua. Este fenómeno único atrae a buceadores de todas partes, que se sumergen para vivir la experiencia de nadar sobre un bosque y capturar fotografías impresionantes, como si fueran imágenes aéreas. Para quienes no
+quieran sumergirse, se puede navegar en un paseo y además el bosque puede apreciarse desde la superficie gracias a la transparencia del Lago Traful. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para
+quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Este rincón especial dio origen al Parque Provincial Copahue, un espacio de naturaleza pura donde la tranquilidad lo envuelve todo. A 1800 msnm, el pequeño poblado invita a recorrerlo a pie, disfrutando de la calma y la energía única de la zona. La experiencia se vive sin apuros, permitiendo
+disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Un espacio donde la espiritualidad y el arte se fusionan en un recorrido único. Este parque ofrece una experiencia visual y emocional en honor a la vida y enseñanzas de Jesús. El Vía Christi, cuyo significado es "Camino de Cristo", presenta 24 estaciones con impactantes esculturas que relatan
+episodios clave de su vida. Las obras, creadas por el artista Alejandro Santana, integran símbolos cristianos con elementos de la cultura mapuche. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para
+quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Todos los circuitos permiten explorar los bosques de lenga, coihue, ñire y descubrir los glaciares, ríos, arroyos, lagunas, turberas, mallines y praderas de altura. La Oficina de Informes de Montaña, en el centro de el Bolsón, brinda información sobre la apertura de cada refugio y el estado de los
+senderos La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan
+mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Se puede realizar esquí alpino, esquí de fondo, freestyle, snowboard, paseos en trineos, motos de nieve y en cuatriciclos con orugas; además de realizar caminatas con raquetas y andar en snow bmx. A su vez, cuenta con estadios de entrenamiento para deportistas de competición. El centro tiene una
+gran infraestructura de servicios como hoteles, restaurantes, escuelas de esquí, venta y alquiler de equipo, shopping con venta de indumentaria, experiencia virtual inmersiva y kids club. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar,
+aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Partiendo desde Puerto Pañuelo, en la península de Llao Llao, es posible realizar distintas navegaciones: -Isla Victoria y recorrer sus senderos -Parque Nacional Arrayanes para visitar el famoso bosque de Arrayanes -Puerto Blest y la Cascada de los Cántaros -Brazo Tristeza y Cascada del Arroyo Frey
+Este tipo de excursiones son recomendadas para toda la familia en embarcaciones cómodas y equipadas durante todo el año. También es posible realizar el cruce andino entre nuestro país y el país vecino de Chile navegando por el Lago Frías. La experiencia se vive sin apuros, permitiendo disfrutar cada
+detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>A bordo de balsas compartidas y con la compañía de guías profesionales, la energía del río se transforma en una vivencia cargada de adrenalina, perfecta para grupos de amigos o planes familiares. A solo 95 kilómetros de la ciudad de Salta, el dique Cabra Corral ofrece mucho más: bungee jumping, ski
+acuático, kayak, rappel y tranquilos paseos en catamarán, un destino de aventura natural. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes
+buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>En San Antonio de los Cobres es posible recorrer el mercado artesanal para ver cómo es el trabajo en los telares, conocer la iglesia San Antonio de Padua y el Museo Regional Andino para aprender sobre la historia y las costumbres de la Puna. También se puede pasear con llamas, compartir un día con
+un típico pastor de la zona, visitar un taller de mujeres artesanas o participar de un taller de artesanías en cerámica. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por
+primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>En medio del desierto es posible conocer los Ojos de Mar, 3 lagunas de origen volcánico en medio de un salar blanco cuyo color varía, según la luz del sol, entre el turquesa y el verde. Resguardan microorganismos milenarios similares a los que dieron origen a la vida en la Tierra. Al pie del volcán
+Incahuasi, la laguna de Santa María es el ambiente natural de flamencos rosados, gallaretas y otras llamativas aves puneñas. La época para los avistajes es entre septiembre y marzo. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y
+relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Impulsarse con el viento a través del kitesurf y el windsurf aquí es perfecto. El dique está enmarcado entre cordones montañosos y cielos azules. Cuenta con paradores gastronómicos, escuelas con instructores y servicios de alquiler de equipos. Es un espectáculo digno de observar, tanto las jornadas
+de prácticas como las de competencias. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja
+recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Se pueden realizar distintas modalidades de kayak como Aguas Blancas, Kayak freestyle y Slalom o Piragüismo. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como
+para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El Parque ofrece diversas modalidades para su recorrido:  Circuito Tradicional: dura aproximadamente 3 horas y permite conocer las geoformas más emblemáticas del sitio, como El Hongo, El Submarino y Cancha de Bochas.  Caminata al Cerro Morado: esta opción que permite ascender a la cima para obtener
+una vista panorámica y apreciar la variedad cromática del paisaje.  Circuitos de Trekking: al Río Salado y a la Quebrada de la Peña en donde se aprecia la imponente geografía marcada por la erosión fluvial y eólica.  Recorrido en Bicicleta: un trayecto de 12 kilómetros por un área de dificultad
+media-alta, para el cual el Parque dispone de bicicletas acondicionadas.  Circuitos Nocturnos: se realizan durante las noches de luna llena.  La localidad de San Agustín del Valle Fértil se encuentra a 73 kilómetros del Parque y cuenta con alojamientos y servicios de gastronomía. La experiencia se
+vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El lugar cuenta con campings, clubes náuticos y un balneario habilitado en temporada de verano. También dispone de áreas con asadores y arboledas que brindan sombra, haciendo posible disfrutar de jornadas completas al aire libre en cualquier época del año. Acampar junto al embalse permite extender
+la estadía y disfrutar de la tranquilidad del entorno, con la posibilidad de admirar un cielo nocturno cargado de estrellas. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por
+primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El Parque Astronómico La Punta es una experiencia única para grandes y chicos, donde el cielo puntano se convierte en escenario de aprendizaje y asombro. La Punta no solo invita a conocer el pasado, sino también a imaginar el futuro desde un rincón pujante de la provincia con un estadio y una
+Universidad. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que
+acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Es frecuente avistar el vuelo de cóndores sobre los cerros que enmarcan el espejo de agua rodeado de molles, algarrobos, talas y chañares.También es posible practicar pesca deportiva, disfrutar de caminatas por escalinatas naturales o capturar postales. El dique abastece de agua para uso humano,
+ganadero y agrícola en las zonas cercanas de la provincia. La tranquilidad del lugar, el aire serrano hacen del dique un lugar perfecto para desconectar y disfrutar del paisaje. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y
+relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Además, a 20 kilómetros de Puerto Deseado y accediendo con una excursión embarcada, el Parque Interjurisdiccional Isla Pingüino es una de las joyas de la zona. Se trata de un área protegida que tiene la única colonia de pingüinos de penacho amarillo de fácil acceso en la Argentina. Sentarse en
+silencio a observarlos en un pequeño islote rocoso rodeado por el océano Atlántico, es una experiencia inolvidable. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera
+vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El trekking sobre hielo se realiza en pequeños grupos junto con dos guías de montaña habilitados y con el equipo necesario: crampones, cascos y arneses. La experiencia es única, caminar sobre el glaciar, entre lagunas azules, grietas, sumideros, cuevas y por momentos por bosque y el marco de los
+cerros. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan
+mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Sendero a la Laguna de los Tres: (25 kilómetros ida y vuelta - dificultad media/alta) llega hasta la base del famoso Cerro Fitz Roy y a la hermosa laguna que está a sus pies. Dentro de este recorrido hay una alternativa intermedia de 8 km ida y vuelta que llega hasta la Laguna Capri, con vistas
+increíbles de los cerros. Sendero a la Laguna Torre: (19 kilómetros ida y vuelta - dificultad baja) va por el valle hasta la Laguna Torre, aunque se puede optar por hacer una caminata de 5 km ida y vuelta que llega hasta un mirador panorámico desde donde se ve el Cerro Torre. La experiencia se vive
+sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El Teatro El Círculo se destaca por su excepcional acústica y su elegante sala con capacidad para 1.550 personas. En sus catacumbas funciona el Museo de Arte Sacro, que alberga obras del escultor Eduardo Barnes. Rosario es también reconocida como cuna de importantes figuras del arte, la música y el
+deporte argentino. Se pueden recorrer espacios vinculados a personalidades como Alberto Olmedo, Roberto Fontanarrosa, Litto Nebbia, Fito Páez y Lionel Messi, cuyos legados se celebran a través de distintos circuitos recorriendo lugares clave de la ciudad. La experiencia se vive sin apuros,
+permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Los paseos en sus diferentes formas permiten apreciar ambas márgenes del río y, por tanto, el peculiar contraste entre el perfil urbano del lado rosarino y el horizonte verde que da inicio a unos 60 kilómetros de delta isleño. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y
+aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Otro imperdible de esta ciudad litoraleña es la Manzana Jesuítica de Santa Fe. Este circuito que forma parte del Camino de los Jesuitas está integrado por el Santuario Nuestra Señora de los Milagros, el más antiguo de la provincia declarado Monumento Histórico Nacional, y que conserva en su interior
+un cuadro milagroso original de 1636; el Colegio Inmaculada Concepción, primer colegio jesuita del país; el antiguo patio de clausura con su capilla doméstica donde vieron transitar al Papa Francisco en sus años de formación como maestro; y por último, en los niveles superiores, el sector del
+Observatorio y Museo de la Manzana Jesuítica de Santa Fe. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una
+actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Termas de Río Hondo está a 73 kilómetros de la ciudad de Santiago del Estero por la ruta nacional 9. Tanto la ciudad de Santiago del Estero como Termas de Río Hondo cuentan con aeropuerto. También hay micros con frecuencias desde varios puntos del país. La experiencia se vive sin apuros, permitiendo
+disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Otra opción imperdible para los fanáticos del mundo automovilístico es recorrer el Museo del Automóvil, ubicado dentro del predio, que posee una colección muy interesante de autos antiguos. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar,
+aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Cada año se realiza en el mes de julio y en el marco de los festejos por el aniversario de la ciudad de Santiago del Estero la "Marcha de los Bombos", idea que surgió del propio "Indio" Froilán y otros amigos, en donde cientos de personas caminan tocando los bombos durante 10 kilómetros, celebrando
+sus tradiciones. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que
+acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Su ubicación y orientación sur generan una excelente calidad de nieve en polvo y brindan las mejores condiciones para practicar estos deportes. Por estas razones, Ushuaia fue declarada Capital Nacional del Esquí de Fondo, una actividad muy popular y tradicional del invierno fueguino. Además, cuenta
+con un snowpark y una pista de patinaje sobre hielo. A su vez, se puede disfrutar de un shopping de montaña y variada gastronomía. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la
+zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Algunas excursiones permiten descender en la isla Karelo o isla H para realizar una caminata breve con vistas panorámicas. También hay salidas hacia la Isla Martillo, hogar estacional de pingüinos magallánicos y la histórica Estancia Harberton, con visita guiada incluida. La experiencia se vive sin
+apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Otro lugar imperdible es la Isla de los Lobos, hogar de una colonia de lobos marinos de un pelo, a la cual se accede mediante excursiones organizadas por prestadores autorizados. Para los aficionados de la observación de aves, la bahía San Sebastián es una excelente opción. Además, Río Grande cuenta
+con varios senderos ideales para caminatas. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja
+recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>El recorrido se puede realizar en vehículo particular gracias a un sistema de cartelería que guía a lo largo de la Ruta por cada taller. Si no, se puede contratar una agencia ya que las distancias entre algunos talleres son largas y los caminos son empedrados y sinuosos. La experiencia se vive sin
+apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Es posible recorrer sus antiguas estructuras, desde la zona residencial hasta la fortaleza en la cima del cerro entre sus pircas, sitios ceremoniales y miles de cardones. La visita además cuenta con el Centro de Interpretación de Quilmes, que ofrece exhibiciones, recursos audiovisuales y táctiles
+para conocer su cultura, costumbres y legado. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es una actividad que deja
+recuerdos y sensaciones que acompañan mucho después del viaje.</t>
+  </si>
+  <si>
+    <t>Rodeado de sierras en un entorno natural único, ofrece además senderos para explorar, aerosillas con vistas panorámicas del cerro Médici y el complejo turístico Puerto Argentino, con lindas vistas panorámicas y propuestas gastronómicas. Los más aventureros pueden realizar senderismo, mountain bike y
+rappel donde se puede explorar el espejo de agua y sus alrededores. La experiencia se vive sin apuros, permitiendo disfrutar cada detalle y aprovechar el tiempo para observar, aprender y relajarse. Ideal tanto para quienes visitan la zona por primera vez como para quienes buscan redescubrirla, es
+una actividad que deja recuerdos y sensaciones que acompañan mucho después del viaje.</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +2200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1094,28 +2246,28 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>273</v>
       </c>
       <c r="G2" t="s">
-        <v>149</v>
+        <v>345</v>
       </c>
       <c r="H2" t="s">
-        <v>179</v>
+        <v>417</v>
       </c>
       <c r="I2" t="s">
-        <v>209</v>
+        <v>489</v>
       </c>
       <c r="J2">
         <v>-34.243617</v>
@@ -1129,28 +2281,28 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>274</v>
       </c>
       <c r="G3" t="s">
-        <v>150</v>
+        <v>346</v>
       </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>418</v>
       </c>
       <c r="I3" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J3">
         <v>-34.920345</v>
@@ -1164,28 +2316,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>275</v>
       </c>
       <c r="G4" t="s">
-        <v>151</v>
+        <v>347</v>
       </c>
       <c r="H4" t="s">
-        <v>181</v>
+        <v>419</v>
       </c>
       <c r="I4" t="s">
-        <v>209</v>
+        <v>489</v>
       </c>
       <c r="J4">
         <v>-34.1825</v>
@@ -1199,28 +2351,28 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>276</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>348</v>
       </c>
       <c r="H5" t="s">
-        <v>182</v>
+        <v>420</v>
       </c>
       <c r="I5" t="s">
-        <v>211</v>
+        <v>491</v>
       </c>
       <c r="J5">
         <v>-34.56972</v>
@@ -1234,28 +2386,28 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>205</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>277</v>
       </c>
       <c r="G6" t="s">
-        <v>153</v>
+        <v>349</v>
       </c>
       <c r="H6" t="s">
-        <v>183</v>
+        <v>421</v>
       </c>
       <c r="I6" t="s">
-        <v>209</v>
+        <v>489</v>
       </c>
       <c r="J6">
         <v>-34.5903</v>
@@ -1269,28 +2421,28 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>206</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>278</v>
       </c>
       <c r="G7" t="s">
-        <v>154</v>
+        <v>350</v>
       </c>
       <c r="H7" t="s">
-        <v>184</v>
+        <v>422</v>
       </c>
       <c r="I7" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J7">
         <v>-34.60117</v>
@@ -1304,28 +2456,28 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>207</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>279</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>351</v>
       </c>
       <c r="H8" t="s">
-        <v>185</v>
+        <v>423</v>
       </c>
       <c r="I8" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J8">
         <v>-28.46957</v>
@@ -1339,28 +2491,28 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>208</v>
       </c>
       <c r="F9" t="s">
-        <v>126</v>
+        <v>280</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>352</v>
       </c>
       <c r="H9" t="s">
-        <v>186</v>
+        <v>424</v>
       </c>
       <c r="I9" t="s">
-        <v>209</v>
+        <v>489</v>
       </c>
       <c r="J9">
         <v>-27.689199</v>
@@ -1374,28 +2526,28 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="F10" t="s">
-        <v>127</v>
+        <v>281</v>
       </c>
       <c r="G10" t="s">
-        <v>157</v>
+        <v>353</v>
       </c>
       <c r="H10" t="s">
-        <v>187</v>
+        <v>425</v>
       </c>
       <c r="I10" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J10">
         <v>-26.79095</v>
@@ -1409,28 +2561,28 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>282</v>
       </c>
       <c r="G11" t="s">
-        <v>158</v>
+        <v>354</v>
       </c>
       <c r="H11" t="s">
-        <v>188</v>
+        <v>426</v>
       </c>
       <c r="I11" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J11">
         <v>-27.315707</v>
@@ -1444,28 +2596,28 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>211</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>283</v>
       </c>
       <c r="G12" t="s">
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>427</v>
       </c>
       <c r="I12" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J12">
         <v>-27.609722</v>
@@ -1479,28 +2631,28 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
+        <v>284</v>
       </c>
       <c r="G13" t="s">
-        <v>160</v>
+        <v>356</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>428</v>
       </c>
       <c r="I13" t="s">
-        <v>211</v>
+        <v>491</v>
       </c>
       <c r="J13">
         <v>-44.04</v>
@@ -1514,28 +2666,28 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>285</v>
       </c>
       <c r="G14" t="s">
-        <v>161</v>
+        <v>357</v>
       </c>
       <c r="H14" t="s">
-        <v>191</v>
+        <v>429</v>
       </c>
       <c r="I14" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J14">
         <v>-42.833061</v>
@@ -1549,28 +2701,28 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>286</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
+        <v>358</v>
       </c>
       <c r="H15" t="s">
-        <v>192</v>
+        <v>430</v>
       </c>
       <c r="I15" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J15">
         <v>-42.91147</v>
@@ -1584,28 +2736,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>287</v>
       </c>
       <c r="G16" t="s">
-        <v>163</v>
+        <v>359</v>
       </c>
       <c r="H16" t="s">
-        <v>193</v>
+        <v>431</v>
       </c>
       <c r="I16" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J16">
         <v>-42.57018</v>
@@ -1619,28 +2771,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>288</v>
       </c>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>360</v>
       </c>
       <c r="H17" t="s">
-        <v>194</v>
+        <v>432</v>
       </c>
       <c r="I17" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J17">
         <v>-31.4124</v>
@@ -1654,28 +2806,28 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>217</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>289</v>
       </c>
       <c r="G18" t="s">
-        <v>165</v>
+        <v>361</v>
       </c>
       <c r="H18" t="s">
-        <v>195</v>
+        <v>433</v>
       </c>
       <c r="I18" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J18">
         <v>-31.715309</v>
@@ -1689,28 +2841,28 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>290</v>
       </c>
       <c r="G19" t="s">
-        <v>166</v>
+        <v>362</v>
       </c>
       <c r="H19" t="s">
-        <v>196</v>
+        <v>434</v>
       </c>
       <c r="I19" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J19">
         <v>-31.653664</v>
@@ -1724,28 +2876,28 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>291</v>
       </c>
       <c r="G20" t="s">
-        <v>167</v>
+        <v>363</v>
       </c>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>435</v>
       </c>
       <c r="I20" t="s">
-        <v>211</v>
+        <v>491</v>
       </c>
       <c r="J20">
         <v>-28.53722</v>
@@ -1759,28 +2911,28 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>220</v>
       </c>
       <c r="F21" t="s">
-        <v>138</v>
+        <v>292</v>
       </c>
       <c r="G21" t="s">
-        <v>168</v>
+        <v>364</v>
       </c>
       <c r="H21" t="s">
-        <v>198</v>
+        <v>436</v>
       </c>
       <c r="I21" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J21">
         <v>-28.39175</v>
@@ -1794,28 +2946,28 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>221</v>
       </c>
       <c r="F22" t="s">
-        <v>139</v>
+        <v>293</v>
       </c>
       <c r="G22" t="s">
-        <v>169</v>
+        <v>365</v>
       </c>
       <c r="H22" t="s">
-        <v>199</v>
+        <v>437</v>
       </c>
       <c r="I22" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J22">
         <v>-29.469768</v>
@@ -1829,28 +2981,28 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>222</v>
       </c>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>294</v>
       </c>
       <c r="G23" t="s">
-        <v>170</v>
+        <v>366</v>
       </c>
       <c r="H23" t="s">
-        <v>200</v>
+        <v>438</v>
       </c>
       <c r="I23" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J23">
         <v>-28.50773</v>
@@ -1864,28 +3016,28 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>295</v>
       </c>
       <c r="G24" t="s">
-        <v>171</v>
+        <v>367</v>
       </c>
       <c r="H24" t="s">
-        <v>201</v>
+        <v>439</v>
       </c>
       <c r="I24" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J24">
         <v>-33.015018</v>
@@ -1899,28 +3051,28 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>224</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>296</v>
       </c>
       <c r="G25" t="s">
-        <v>172</v>
+        <v>368</v>
       </c>
       <c r="H25" t="s">
-        <v>202</v>
+        <v>440</v>
       </c>
       <c r="I25" t="s">
-        <v>212</v>
+        <v>492</v>
       </c>
       <c r="J25">
         <v>-30.223096</v>
@@ -1934,28 +3086,28 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>225</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>297</v>
       </c>
       <c r="G26" t="s">
-        <v>173</v>
+        <v>369</v>
       </c>
       <c r="H26" t="s">
-        <v>203</v>
+        <v>441</v>
       </c>
       <c r="I26" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J26">
         <v>-31.88216</v>
@@ -1969,28 +3121,28 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>298</v>
       </c>
       <c r="G27" t="s">
-        <v>174</v>
+        <v>370</v>
       </c>
       <c r="H27" t="s">
-        <v>204</v>
+        <v>442</v>
       </c>
       <c r="I27" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J27">
         <v>-26.185201</v>
@@ -2004,28 +3156,28 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
+        <v>227</v>
       </c>
       <c r="F28" t="s">
-        <v>145</v>
+        <v>299</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>371</v>
       </c>
       <c r="H28" t="s">
-        <v>205</v>
+        <v>443</v>
       </c>
       <c r="I28" t="s">
-        <v>212</v>
+        <v>492</v>
       </c>
       <c r="J28">
         <v>-25.12965</v>
@@ -2039,28 +3191,28 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>228</v>
       </c>
       <c r="F29" t="s">
-        <v>146</v>
+        <v>300</v>
       </c>
       <c r="G29" t="s">
-        <v>176</v>
+        <v>372</v>
       </c>
       <c r="H29" t="s">
-        <v>206</v>
+        <v>444</v>
       </c>
       <c r="I29" t="s">
-        <v>212</v>
+        <v>492</v>
       </c>
       <c r="J29">
         <v>-24.431834</v>
@@ -2074,28 +3226,28 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="E30" t="s">
-        <v>117</v>
+        <v>229</v>
       </c>
       <c r="F30" t="s">
-        <v>147</v>
+        <v>301</v>
       </c>
       <c r="G30" t="s">
-        <v>177</v>
+        <v>373</v>
       </c>
       <c r="H30" t="s">
-        <v>207</v>
+        <v>445</v>
       </c>
       <c r="I30" t="s">
-        <v>210</v>
+        <v>490</v>
       </c>
       <c r="J30">
         <v>-23.669147</v>
@@ -2109,34 +3261,1504 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
+        <v>230</v>
       </c>
       <c r="F31" t="s">
-        <v>148</v>
+        <v>302</v>
       </c>
       <c r="G31" t="s">
-        <v>178</v>
+        <v>374</v>
       </c>
       <c r="H31" t="s">
-        <v>208</v>
+        <v>446</v>
       </c>
       <c r="I31" t="s">
-        <v>212</v>
+        <v>492</v>
       </c>
       <c r="J31">
         <v>-23.730833</v>
       </c>
       <c r="K31">
         <v>-65.979722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32" t="s">
+        <v>303</v>
+      </c>
+      <c r="G32" t="s">
+        <v>375</v>
+      </c>
+      <c r="H32" t="s">
+        <v>447</v>
+      </c>
+      <c r="I32" t="s">
+        <v>493</v>
+      </c>
+      <c r="J32">
+        <v>-36.2297</v>
+      </c>
+      <c r="K32">
+        <v>-66.94370000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" t="s">
+        <v>304</v>
+      </c>
+      <c r="G33" t="s">
+        <v>376</v>
+      </c>
+      <c r="H33" t="s">
+        <v>448</v>
+      </c>
+      <c r="I33" t="s">
+        <v>494</v>
+      </c>
+      <c r="J33">
+        <v>-37.1206</v>
+      </c>
+      <c r="K33">
+        <v>-63.5983</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" t="s">
+        <v>305</v>
+      </c>
+      <c r="G34" t="s">
+        <v>377</v>
+      </c>
+      <c r="H34" t="s">
+        <v>449</v>
+      </c>
+      <c r="I34" t="s">
+        <v>495</v>
+      </c>
+      <c r="J34">
+        <v>-36.9169</v>
+      </c>
+      <c r="K34">
+        <v>-64.28360000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" t="s">
+        <v>306</v>
+      </c>
+      <c r="G35" t="s">
+        <v>378</v>
+      </c>
+      <c r="H35" t="s">
+        <v>450</v>
+      </c>
+      <c r="I35" t="s">
+        <v>496</v>
+      </c>
+      <c r="J35">
+        <v>-29.4131</v>
+      </c>
+      <c r="K35">
+        <v>-66.8558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" t="s">
+        <v>307</v>
+      </c>
+      <c r="G36" t="s">
+        <v>379</v>
+      </c>
+      <c r="H36" t="s">
+        <v>451</v>
+      </c>
+      <c r="I36" t="s">
+        <v>497</v>
+      </c>
+      <c r="J36">
+        <v>-29.4131</v>
+      </c>
+      <c r="K36">
+        <v>-66.8558</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" t="s">
+        <v>236</v>
+      </c>
+      <c r="F37" t="s">
+        <v>308</v>
+      </c>
+      <c r="G37" t="s">
+        <v>380</v>
+      </c>
+      <c r="H37" t="s">
+        <v>452</v>
+      </c>
+      <c r="I37" t="s">
+        <v>498</v>
+      </c>
+      <c r="J37">
+        <v>-29.4131</v>
+      </c>
+      <c r="K37">
+        <v>-66.8558</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" t="s">
+        <v>309</v>
+      </c>
+      <c r="G38" t="s">
+        <v>381</v>
+      </c>
+      <c r="H38" t="s">
+        <v>453</v>
+      </c>
+      <c r="I38" t="s">
+        <v>499</v>
+      </c>
+      <c r="J38">
+        <v>-32.8895</v>
+      </c>
+      <c r="K38">
+        <v>-68.8458</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" t="s">
+        <v>310</v>
+      </c>
+      <c r="G39" t="s">
+        <v>382</v>
+      </c>
+      <c r="H39" t="s">
+        <v>454</v>
+      </c>
+      <c r="I39" t="s">
+        <v>500</v>
+      </c>
+      <c r="J39">
+        <v>-32.8895</v>
+      </c>
+      <c r="K39">
+        <v>-68.8458</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" t="s">
+        <v>311</v>
+      </c>
+      <c r="G40" t="s">
+        <v>383</v>
+      </c>
+      <c r="H40" t="s">
+        <v>455</v>
+      </c>
+      <c r="I40" t="s">
+        <v>501</v>
+      </c>
+      <c r="J40">
+        <v>-32.8895</v>
+      </c>
+      <c r="K40">
+        <v>-68.8458</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" t="s">
+        <v>312</v>
+      </c>
+      <c r="G41" t="s">
+        <v>384</v>
+      </c>
+      <c r="H41" t="s">
+        <v>456</v>
+      </c>
+      <c r="I41" t="s">
+        <v>502</v>
+      </c>
+      <c r="J41">
+        <v>-27.3621</v>
+      </c>
+      <c r="K41">
+        <v>-55.9008</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" t="s">
+        <v>241</v>
+      </c>
+      <c r="F42" t="s">
+        <v>313</v>
+      </c>
+      <c r="G42" t="s">
+        <v>385</v>
+      </c>
+      <c r="H42" t="s">
+        <v>457</v>
+      </c>
+      <c r="I42" t="s">
+        <v>503</v>
+      </c>
+      <c r="J42">
+        <v>-27.3621</v>
+      </c>
+      <c r="K42">
+        <v>-55.9008</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" t="s">
+        <v>242</v>
+      </c>
+      <c r="F43" t="s">
+        <v>314</v>
+      </c>
+      <c r="G43" t="s">
+        <v>386</v>
+      </c>
+      <c r="H43" t="s">
+        <v>458</v>
+      </c>
+      <c r="I43" t="s">
+        <v>504</v>
+      </c>
+      <c r="J43">
+        <v>-27.3621</v>
+      </c>
+      <c r="K43">
+        <v>-55.9008</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" t="s">
+        <v>243</v>
+      </c>
+      <c r="F44" t="s">
+        <v>315</v>
+      </c>
+      <c r="G44" t="s">
+        <v>387</v>
+      </c>
+      <c r="H44" t="s">
+        <v>459</v>
+      </c>
+      <c r="I44" t="s">
+        <v>505</v>
+      </c>
+      <c r="J44">
+        <v>-38.9516</v>
+      </c>
+      <c r="K44">
+        <v>-68.0591</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" t="s">
+        <v>244</v>
+      </c>
+      <c r="F45" t="s">
+        <v>316</v>
+      </c>
+      <c r="G45" t="s">
+        <v>388</v>
+      </c>
+      <c r="H45" t="s">
+        <v>460</v>
+      </c>
+      <c r="I45" t="s">
+        <v>506</v>
+      </c>
+      <c r="J45">
+        <v>-38.9516</v>
+      </c>
+      <c r="K45">
+        <v>-68.0591</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" t="s">
+        <v>245</v>
+      </c>
+      <c r="F46" t="s">
+        <v>317</v>
+      </c>
+      <c r="G46" t="s">
+        <v>389</v>
+      </c>
+      <c r="H46" t="s">
+        <v>461</v>
+      </c>
+      <c r="I46" t="s">
+        <v>507</v>
+      </c>
+      <c r="J46">
+        <v>-38.9516</v>
+      </c>
+      <c r="K46">
+        <v>-68.0591</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" t="s">
+        <v>246</v>
+      </c>
+      <c r="F47" t="s">
+        <v>318</v>
+      </c>
+      <c r="G47" t="s">
+        <v>390</v>
+      </c>
+      <c r="H47" t="s">
+        <v>462</v>
+      </c>
+      <c r="I47" t="s">
+        <v>508</v>
+      </c>
+      <c r="J47">
+        <v>-41.1335</v>
+      </c>
+      <c r="K47">
+        <v>-71.3103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F48" t="s">
+        <v>319</v>
+      </c>
+      <c r="G48" t="s">
+        <v>391</v>
+      </c>
+      <c r="H48" t="s">
+        <v>463</v>
+      </c>
+      <c r="I48" t="s">
+        <v>509</v>
+      </c>
+      <c r="J48">
+        <v>-41.1335</v>
+      </c>
+      <c r="K48">
+        <v>-71.3103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" t="s">
+        <v>248</v>
+      </c>
+      <c r="F49" t="s">
+        <v>320</v>
+      </c>
+      <c r="G49" t="s">
+        <v>392</v>
+      </c>
+      <c r="H49" t="s">
+        <v>464</v>
+      </c>
+      <c r="I49" t="s">
+        <v>510</v>
+      </c>
+      <c r="J49">
+        <v>-41.1335</v>
+      </c>
+      <c r="K49">
+        <v>-71.3103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" t="s">
+        <v>177</v>
+      </c>
+      <c r="E50" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" t="s">
+        <v>321</v>
+      </c>
+      <c r="G50" t="s">
+        <v>393</v>
+      </c>
+      <c r="H50" t="s">
+        <v>465</v>
+      </c>
+      <c r="I50" t="s">
+        <v>511</v>
+      </c>
+      <c r="J50">
+        <v>-24.7829</v>
+      </c>
+      <c r="K50">
+        <v>-65.42319999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" t="s">
+        <v>178</v>
+      </c>
+      <c r="E51" t="s">
+        <v>250</v>
+      </c>
+      <c r="F51" t="s">
+        <v>322</v>
+      </c>
+      <c r="G51" t="s">
+        <v>394</v>
+      </c>
+      <c r="H51" t="s">
+        <v>466</v>
+      </c>
+      <c r="I51" t="s">
+        <v>512</v>
+      </c>
+      <c r="J51">
+        <v>-24.7829</v>
+      </c>
+      <c r="K51">
+        <v>-65.42319999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" t="s">
+        <v>179</v>
+      </c>
+      <c r="E52" t="s">
+        <v>251</v>
+      </c>
+      <c r="F52" t="s">
+        <v>323</v>
+      </c>
+      <c r="G52" t="s">
+        <v>395</v>
+      </c>
+      <c r="H52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I52" t="s">
+        <v>513</v>
+      </c>
+      <c r="J52">
+        <v>-24.7829</v>
+      </c>
+      <c r="K52">
+        <v>-65.42319999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>180</v>
+      </c>
+      <c r="E53" t="s">
+        <v>252</v>
+      </c>
+      <c r="F53" t="s">
+        <v>324</v>
+      </c>
+      <c r="G53" t="s">
+        <v>396</v>
+      </c>
+      <c r="H53" t="s">
+        <v>468</v>
+      </c>
+      <c r="I53" t="s">
+        <v>514</v>
+      </c>
+      <c r="J53">
+        <v>-31.5375</v>
+      </c>
+      <c r="K53">
+        <v>-68.5364</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" t="s">
+        <v>253</v>
+      </c>
+      <c r="F54" t="s">
+        <v>325</v>
+      </c>
+      <c r="G54" t="s">
+        <v>397</v>
+      </c>
+      <c r="H54" t="s">
+        <v>469</v>
+      </c>
+      <c r="I54" t="s">
+        <v>515</v>
+      </c>
+      <c r="J54">
+        <v>-31.5375</v>
+      </c>
+      <c r="K54">
+        <v>-68.5364</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55" t="s">
+        <v>254</v>
+      </c>
+      <c r="F55" t="s">
+        <v>326</v>
+      </c>
+      <c r="G55" t="s">
+        <v>398</v>
+      </c>
+      <c r="H55" t="s">
+        <v>470</v>
+      </c>
+      <c r="I55" t="s">
+        <v>516</v>
+      </c>
+      <c r="J55">
+        <v>-31.5375</v>
+      </c>
+      <c r="K55">
+        <v>-68.5364</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E56" t="s">
+        <v>255</v>
+      </c>
+      <c r="F56" t="s">
+        <v>327</v>
+      </c>
+      <c r="G56" t="s">
+        <v>399</v>
+      </c>
+      <c r="H56" t="s">
+        <v>471</v>
+      </c>
+      <c r="I56" t="s">
+        <v>517</v>
+      </c>
+      <c r="J56">
+        <v>-33.3017</v>
+      </c>
+      <c r="K56">
+        <v>-66.3378</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>184</v>
+      </c>
+      <c r="E57" t="s">
+        <v>256</v>
+      </c>
+      <c r="F57" t="s">
+        <v>328</v>
+      </c>
+      <c r="G57" t="s">
+        <v>400</v>
+      </c>
+      <c r="H57" t="s">
+        <v>472</v>
+      </c>
+      <c r="I57" t="s">
+        <v>518</v>
+      </c>
+      <c r="J57">
+        <v>-33.3017</v>
+      </c>
+      <c r="K57">
+        <v>-66.3378</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" t="s">
+        <v>257</v>
+      </c>
+      <c r="F58" t="s">
+        <v>329</v>
+      </c>
+      <c r="G58" t="s">
+        <v>401</v>
+      </c>
+      <c r="H58" t="s">
+        <v>473</v>
+      </c>
+      <c r="I58" t="s">
+        <v>519</v>
+      </c>
+      <c r="J58">
+        <v>-33.3017</v>
+      </c>
+      <c r="K58">
+        <v>-66.3378</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" t="s">
+        <v>186</v>
+      </c>
+      <c r="E59" t="s">
+        <v>258</v>
+      </c>
+      <c r="F59" t="s">
+        <v>330</v>
+      </c>
+      <c r="G59" t="s">
+        <v>402</v>
+      </c>
+      <c r="H59" t="s">
+        <v>474</v>
+      </c>
+      <c r="I59" t="s">
+        <v>520</v>
+      </c>
+      <c r="J59">
+        <v>-51.623</v>
+      </c>
+      <c r="K59">
+        <v>-69.21680000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" t="s">
+        <v>259</v>
+      </c>
+      <c r="F60" t="s">
+        <v>331</v>
+      </c>
+      <c r="G60" t="s">
+        <v>403</v>
+      </c>
+      <c r="H60" t="s">
+        <v>475</v>
+      </c>
+      <c r="I60" t="s">
+        <v>521</v>
+      </c>
+      <c r="J60">
+        <v>-51.623</v>
+      </c>
+      <c r="K60">
+        <v>-69.21680000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D61" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" t="s">
+        <v>260</v>
+      </c>
+      <c r="F61" t="s">
+        <v>332</v>
+      </c>
+      <c r="G61" t="s">
+        <v>404</v>
+      </c>
+      <c r="H61" t="s">
+        <v>476</v>
+      </c>
+      <c r="I61" t="s">
+        <v>522</v>
+      </c>
+      <c r="J61">
+        <v>-51.623</v>
+      </c>
+      <c r="K61">
+        <v>-69.21680000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" t="s">
+        <v>261</v>
+      </c>
+      <c r="F62" t="s">
+        <v>333</v>
+      </c>
+      <c r="G62" t="s">
+        <v>405</v>
+      </c>
+      <c r="H62" t="s">
+        <v>477</v>
+      </c>
+      <c r="I62" t="s">
+        <v>523</v>
+      </c>
+      <c r="J62">
+        <v>-31.6333</v>
+      </c>
+      <c r="K62">
+        <v>-60.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63" t="s">
+        <v>262</v>
+      </c>
+      <c r="F63" t="s">
+        <v>334</v>
+      </c>
+      <c r="G63" t="s">
+        <v>406</v>
+      </c>
+      <c r="H63" t="s">
+        <v>478</v>
+      </c>
+      <c r="I63" t="s">
+        <v>524</v>
+      </c>
+      <c r="J63">
+        <v>-31.6333</v>
+      </c>
+      <c r="K63">
+        <v>-60.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" t="s">
+        <v>191</v>
+      </c>
+      <c r="E64" t="s">
+        <v>263</v>
+      </c>
+      <c r="F64" t="s">
+        <v>335</v>
+      </c>
+      <c r="G64" t="s">
+        <v>407</v>
+      </c>
+      <c r="H64" t="s">
+        <v>479</v>
+      </c>
+      <c r="I64" t="s">
+        <v>525</v>
+      </c>
+      <c r="J64">
+        <v>-31.6333</v>
+      </c>
+      <c r="K64">
+        <v>-60.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" t="s">
+        <v>264</v>
+      </c>
+      <c r="F65" t="s">
+        <v>336</v>
+      </c>
+      <c r="G65" t="s">
+        <v>408</v>
+      </c>
+      <c r="H65" t="s">
+        <v>480</v>
+      </c>
+      <c r="I65" t="s">
+        <v>526</v>
+      </c>
+      <c r="J65">
+        <v>-27.7951</v>
+      </c>
+      <c r="K65">
+        <v>-64.2615</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" t="s">
+        <v>193</v>
+      </c>
+      <c r="E66" t="s">
+        <v>265</v>
+      </c>
+      <c r="F66" t="s">
+        <v>337</v>
+      </c>
+      <c r="G66" t="s">
+        <v>409</v>
+      </c>
+      <c r="H66" t="s">
+        <v>481</v>
+      </c>
+      <c r="I66" t="s">
+        <v>527</v>
+      </c>
+      <c r="J66">
+        <v>-27.7951</v>
+      </c>
+      <c r="K66">
+        <v>-64.2615</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" t="s">
+        <v>124</v>
+      </c>
+      <c r="D67" t="s">
+        <v>194</v>
+      </c>
+      <c r="E67" t="s">
+        <v>266</v>
+      </c>
+      <c r="F67" t="s">
+        <v>338</v>
+      </c>
+      <c r="G67" t="s">
+        <v>410</v>
+      </c>
+      <c r="H67" t="s">
+        <v>482</v>
+      </c>
+      <c r="I67" t="s">
+        <v>528</v>
+      </c>
+      <c r="J67">
+        <v>-27.7951</v>
+      </c>
+      <c r="K67">
+        <v>-64.2615</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" t="s">
+        <v>195</v>
+      </c>
+      <c r="E68" t="s">
+        <v>267</v>
+      </c>
+      <c r="F68" t="s">
+        <v>339</v>
+      </c>
+      <c r="G68" t="s">
+        <v>411</v>
+      </c>
+      <c r="H68" t="s">
+        <v>483</v>
+      </c>
+      <c r="I68" t="s">
+        <v>529</v>
+      </c>
+      <c r="J68">
+        <v>-54.8019</v>
+      </c>
+      <c r="K68">
+        <v>-68.303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" t="s">
+        <v>126</v>
+      </c>
+      <c r="D69" t="s">
+        <v>196</v>
+      </c>
+      <c r="E69" t="s">
+        <v>268</v>
+      </c>
+      <c r="F69" t="s">
+        <v>340</v>
+      </c>
+      <c r="G69" t="s">
+        <v>412</v>
+      </c>
+      <c r="H69" t="s">
+        <v>484</v>
+      </c>
+      <c r="I69" t="s">
+        <v>530</v>
+      </c>
+      <c r="J69">
+        <v>-54.8019</v>
+      </c>
+      <c r="K69">
+        <v>-68.303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" t="s">
+        <v>127</v>
+      </c>
+      <c r="D70" t="s">
+        <v>197</v>
+      </c>
+      <c r="E70" t="s">
+        <v>269</v>
+      </c>
+      <c r="F70" t="s">
+        <v>341</v>
+      </c>
+      <c r="G70" t="s">
+        <v>413</v>
+      </c>
+      <c r="H70" t="s">
+        <v>485</v>
+      </c>
+      <c r="I70" t="s">
+        <v>531</v>
+      </c>
+      <c r="J70">
+        <v>-54.8019</v>
+      </c>
+      <c r="K70">
+        <v>-68.303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s">
+        <v>128</v>
+      </c>
+      <c r="D71" t="s">
+        <v>198</v>
+      </c>
+      <c r="E71" t="s">
+        <v>270</v>
+      </c>
+      <c r="F71" t="s">
+        <v>342</v>
+      </c>
+      <c r="G71" t="s">
+        <v>414</v>
+      </c>
+      <c r="H71" t="s">
+        <v>486</v>
+      </c>
+      <c r="I71" t="s">
+        <v>532</v>
+      </c>
+      <c r="J71">
+        <v>-26.8241</v>
+      </c>
+      <c r="K71">
+        <v>-65.2226</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" t="s">
+        <v>129</v>
+      </c>
+      <c r="D72" t="s">
+        <v>199</v>
+      </c>
+      <c r="E72" t="s">
+        <v>271</v>
+      </c>
+      <c r="F72" t="s">
+        <v>343</v>
+      </c>
+      <c r="G72" t="s">
+        <v>415</v>
+      </c>
+      <c r="H72" t="s">
+        <v>487</v>
+      </c>
+      <c r="I72" t="s">
+        <v>533</v>
+      </c>
+      <c r="J72">
+        <v>-26.8241</v>
+      </c>
+      <c r="K72">
+        <v>-65.2226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" t="s">
+        <v>130</v>
+      </c>
+      <c r="D73" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" t="s">
+        <v>272</v>
+      </c>
+      <c r="F73" t="s">
+        <v>344</v>
+      </c>
+      <c r="G73" t="s">
+        <v>416</v>
+      </c>
+      <c r="H73" t="s">
+        <v>488</v>
+      </c>
+      <c r="I73" t="s">
+        <v>534</v>
+      </c>
+      <c r="J73">
+        <v>-26.8241</v>
+      </c>
+      <c r="K73">
+        <v>-65.2226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>